<commit_message>
Very basic character gameplay concept added
</commit_message>
<xml_diff>
--- a/Documents/Balance.xlsx
+++ b/Documents/Balance.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13275" tabRatio="462" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13275" tabRatio="462" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Analysis" sheetId="3" r:id="rId1"/>
     <sheet name="Constants" sheetId="4" r:id="rId2"/>
     <sheet name="Example_Map" sheetId="2" r:id="rId3"/>
     <sheet name="Average_Character_Template" sheetId="1" r:id="rId4"/>
+    <sheet name="Tactician" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="58">
   <si>
     <t>Width:</t>
   </si>
@@ -104,9 +105,6 @@
     <t>(3-5, random?) Rounds</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
     <t>Score pickups collected</t>
   </si>
   <si>
@@ -146,9 +144,6 @@
     <t>Height Change Per Round Min</t>
   </si>
   <si>
-    <t>Tooltop:</t>
-  </si>
-  <si>
     <t>Dev. Notes:</t>
   </si>
   <si>
@@ -168,6 +163,45 @@
   </si>
   <si>
     <t>{Type}</t>
+  </si>
+  <si>
+    <t>Tooltip:</t>
+  </si>
+  <si>
+    <t>Relocate Turret</t>
+  </si>
+  <si>
+    <t>Place Turret</t>
+  </si>
+  <si>
+    <t>Moves the turret to target location within {P1} tiles distance of it's current position.</t>
+  </si>
+  <si>
+    <t>3 per Tile</t>
+  </si>
+  <si>
+    <t>Places a turret at target location within {P1} tiles distance. The turret has {P2} hitpoints and damage done to it counts toward highscore. While the turret is active, this ability is replaced by 'Relocate Turret'.</t>
+  </si>
+  <si>
+    <t>Actions per Turn:</t>
+  </si>
+  <si>
+    <t>Onclass Offensive</t>
+  </si>
+  <si>
+    <t>Zap</t>
+  </si>
+  <si>
+    <t>Onclass Defensive</t>
+  </si>
+  <si>
+    <t>Overcharge</t>
+  </si>
+  <si>
+    <t>Pushes all living objects {P1} tiles away from both the character and the turret. Enemies affected by this ability take {P2} damage (+50% if hit by both Overcharges).</t>
+  </si>
+  <si>
+    <t>Charges both the character's and the turrets weapon to fire towards target location within {P1} tiles distance. All enemies on tiles which are touched by the direct line drawn between origin and target take {P2} damage (+50% if hit by both shots).</t>
   </si>
 </sst>
 </file>
@@ -447,9 +481,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -491,56 +522,68 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -551,32 +594,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -900,8 +934,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:3" x14ac:dyDescent="0.25">
@@ -909,27 +943,27 @@
       <c r="C1" s="6"/>
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="14"/>
+      <c r="B2" s="13"/>
       <c r="C2" s="3"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="14"/>
+      <c r="B3" s="13"/>
       <c r="C3" s="3"/>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="14"/>
+      <c r="B4" s="13"/>
       <c r="C4" s="3"/>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="14"/>
+      <c r="B5" s="13"/>
       <c r="C5" s="3"/>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="14"/>
+      <c r="B6" s="13"/>
       <c r="C6" s="3"/>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="14"/>
+      <c r="B7" s="13"/>
       <c r="C7" s="9"/>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
@@ -942,20 +976,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -993,11 +1027,11 @@
       <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>25</v>
+      <c r="B3" s="36">
+        <v>3</v>
       </c>
       <c r="C3" t="s">
         <v>24</v>
@@ -1011,8 +1045,8 @@
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
-        <v>34</v>
+      <c r="A4" s="14" t="s">
+        <v>33</v>
       </c>
       <c r="B4" s="1">
         <v>2</v>
@@ -1026,8 +1060,8 @@
       <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
-        <v>35</v>
+      <c r="A5" s="14" t="s">
+        <v>34</v>
       </c>
       <c r="B5" s="1">
         <v>6</v>
@@ -1041,8 +1075,8 @@
       <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
-        <v>36</v>
+      <c r="A6" s="14" t="s">
+        <v>35</v>
       </c>
       <c r="B6" s="1">
         <v>0</v>
@@ -1056,14 +1090,14 @@
       <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
-        <v>38</v>
+      <c r="A7" s="14" t="s">
+        <v>37</v>
       </c>
       <c r="B7" s="1">
         <v>-2</v>
       </c>
       <c r="E7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F7" s="7">
         <v>200</v>
@@ -1071,13 +1105,21 @@
       <c r="G7" s="9"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
-        <v>37</v>
+      <c r="A8" s="14" t="s">
+        <v>36</v>
       </c>
       <c r="B8" s="1">
         <v>2</v>
       </c>
       <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="1">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1094,8 +1136,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="13" width="2.375" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="13" width="2.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -1125,359 +1167,359 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="25">
+        <v>32</v>
+      </c>
+      <c r="D6" s="24">
         <v>0</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="24">
         <v>0</v>
       </c>
-      <c r="F6" s="26">
+      <c r="F6" s="25">
         <v>1</v>
       </c>
-      <c r="G6" s="27">
-        <v>2</v>
-      </c>
-      <c r="H6" s="28">
+      <c r="G6" s="26">
+        <v>2</v>
+      </c>
+      <c r="H6" s="27">
         <v>3</v>
       </c>
-      <c r="I6" s="27">
-        <v>2</v>
-      </c>
-      <c r="J6" s="26">
+      <c r="I6" s="26">
+        <v>2</v>
+      </c>
+      <c r="J6" s="25">
         <v>1</v>
       </c>
-      <c r="K6" s="28">
+      <c r="K6" s="27">
         <v>3</v>
       </c>
-      <c r="L6" s="29">
+      <c r="L6" s="28">
         <v>6</v>
       </c>
-      <c r="M6" s="29">
+      <c r="M6" s="28">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="19">
+      <c r="A7" s="18">
         <v>0</v>
       </c>
-      <c r="D7" s="25">
+      <c r="D7" s="24">
         <v>0</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="24">
         <v>0</v>
       </c>
-      <c r="F7" s="26">
+      <c r="F7" s="25">
         <v>1</v>
       </c>
-      <c r="G7" s="27">
-        <v>2</v>
-      </c>
-      <c r="H7" s="28">
+      <c r="G7" s="26">
+        <v>2</v>
+      </c>
+      <c r="H7" s="27">
         <v>3</v>
       </c>
-      <c r="I7" s="26">
+      <c r="I7" s="25">
         <v>1</v>
       </c>
-      <c r="J7" s="26">
+      <c r="J7" s="25">
         <v>1</v>
       </c>
-      <c r="K7" s="26">
+      <c r="K7" s="25">
         <v>1</v>
       </c>
-      <c r="L7" s="29">
+      <c r="L7" s="28">
         <v>6</v>
       </c>
-      <c r="M7" s="31">
+      <c r="M7" s="30">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="17">
+      <c r="A8" s="16">
         <v>1</v>
       </c>
-      <c r="D8" s="27">
-        <v>2</v>
-      </c>
-      <c r="E8" s="26">
+      <c r="D8" s="26">
+        <v>2</v>
+      </c>
+      <c r="E8" s="25">
         <v>1</v>
       </c>
-      <c r="F8" s="26">
+      <c r="F8" s="25">
         <v>1</v>
       </c>
-      <c r="G8" s="28">
+      <c r="G8" s="27">
         <v>3</v>
       </c>
-      <c r="H8" s="28">
+      <c r="H8" s="27">
         <v>3</v>
       </c>
-      <c r="I8" s="27">
-        <v>2</v>
-      </c>
-      <c r="J8" s="30">
+      <c r="I8" s="26">
+        <v>2</v>
+      </c>
+      <c r="J8" s="29">
         <v>4</v>
       </c>
-      <c r="K8" s="30">
+      <c r="K8" s="29">
         <v>4</v>
       </c>
-      <c r="L8" s="28">
+      <c r="L8" s="27">
         <v>3</v>
       </c>
-      <c r="M8" s="30">
+      <c r="M8" s="29">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="18">
-        <v>2</v>
-      </c>
-      <c r="D9" s="27">
-        <v>2</v>
-      </c>
-      <c r="E9" s="27">
-        <v>2</v>
-      </c>
-      <c r="F9" s="26">
+      <c r="A9" s="17">
+        <v>2</v>
+      </c>
+      <c r="D9" s="26">
+        <v>2</v>
+      </c>
+      <c r="E9" s="26">
+        <v>2</v>
+      </c>
+      <c r="F9" s="25">
         <v>1</v>
       </c>
-      <c r="G9" s="30">
+      <c r="G9" s="29">
         <v>4</v>
       </c>
-      <c r="H9" s="27">
-        <v>2</v>
-      </c>
-      <c r="I9" s="27">
-        <v>2</v>
-      </c>
-      <c r="J9" s="29">
+      <c r="H9" s="26">
+        <v>2</v>
+      </c>
+      <c r="I9" s="26">
+        <v>2</v>
+      </c>
+      <c r="J9" s="28">
         <v>6</v>
       </c>
-      <c r="K9" s="31">
+      <c r="K9" s="30">
         <v>5</v>
       </c>
-      <c r="L9" s="28">
+      <c r="L9" s="27">
         <v>3</v>
       </c>
-      <c r="M9" s="27">
+      <c r="M9" s="26">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="20">
+      <c r="A10" s="19">
         <v>3</v>
       </c>
-      <c r="D10" s="27">
-        <v>2</v>
-      </c>
-      <c r="E10" s="27">
-        <v>2</v>
-      </c>
-      <c r="F10" s="25">
+      <c r="D10" s="26">
+        <v>2</v>
+      </c>
+      <c r="E10" s="26">
+        <v>2</v>
+      </c>
+      <c r="F10" s="24">
         <v>0</v>
       </c>
-      <c r="G10" s="30">
+      <c r="G10" s="29">
         <v>4</v>
       </c>
-      <c r="H10" s="30">
+      <c r="H10" s="29">
         <v>4</v>
       </c>
-      <c r="I10" s="28">
+      <c r="I10" s="27">
         <v>3</v>
       </c>
-      <c r="J10" s="28">
+      <c r="J10" s="27">
         <v>3</v>
       </c>
-      <c r="K10" s="27">
-        <v>2</v>
-      </c>
-      <c r="L10" s="27">
-        <v>2</v>
-      </c>
-      <c r="M10" s="27">
+      <c r="K10" s="26">
+        <v>2</v>
+      </c>
+      <c r="L10" s="26">
+        <v>2</v>
+      </c>
+      <c r="M10" s="26">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="21">
+      <c r="A11" s="20">
         <v>4</v>
       </c>
-      <c r="D11" s="27">
-        <v>2</v>
-      </c>
-      <c r="E11" s="25">
+      <c r="D11" s="26">
+        <v>2</v>
+      </c>
+      <c r="E11" s="24">
         <v>0</v>
       </c>
-      <c r="F11" s="25">
+      <c r="F11" s="24">
         <v>0</v>
       </c>
-      <c r="G11" s="31">
+      <c r="G11" s="30">
         <v>5</v>
       </c>
-      <c r="H11" s="29">
+      <c r="H11" s="28">
         <v>6</v>
       </c>
-      <c r="I11" s="28">
+      <c r="I11" s="27">
         <v>3</v>
       </c>
-      <c r="J11" s="28">
+      <c r="J11" s="27">
         <v>3</v>
       </c>
-      <c r="K11" s="28">
+      <c r="K11" s="27">
         <v>3</v>
       </c>
-      <c r="L11" s="27">
-        <v>2</v>
-      </c>
-      <c r="M11" s="27">
+      <c r="L11" s="26">
+        <v>2</v>
+      </c>
+      <c r="M11" s="26">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="16">
+      <c r="A12" s="15">
         <v>5</v>
       </c>
-      <c r="D12" s="28">
+      <c r="D12" s="27">
         <v>3</v>
       </c>
-      <c r="E12" s="28">
+      <c r="E12" s="27">
         <v>3</v>
       </c>
-      <c r="F12" s="30">
+      <c r="F12" s="29">
         <v>4</v>
       </c>
-      <c r="G12" s="31">
+      <c r="G12" s="30">
         <v>5</v>
       </c>
-      <c r="H12" s="27">
-        <v>2</v>
-      </c>
-      <c r="I12" s="27">
-        <v>2</v>
-      </c>
-      <c r="J12" s="30">
+      <c r="H12" s="26">
+        <v>2</v>
+      </c>
+      <c r="I12" s="26">
+        <v>2</v>
+      </c>
+      <c r="J12" s="29">
         <v>4</v>
       </c>
-      <c r="K12" s="30">
+      <c r="K12" s="29">
         <v>4</v>
       </c>
-      <c r="L12" s="26">
+      <c r="L12" s="25">
         <v>1</v>
       </c>
-      <c r="M12" s="26">
+      <c r="M12" s="25">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="22">
+      <c r="A13" s="21">
         <v>6</v>
       </c>
-      <c r="D13" s="28">
+      <c r="D13" s="27">
         <v>3</v>
       </c>
-      <c r="E13" s="28">
+      <c r="E13" s="27">
         <v>3</v>
       </c>
-      <c r="F13" s="28">
+      <c r="F13" s="27">
         <v>3</v>
       </c>
-      <c r="G13" s="27">
-        <v>2</v>
-      </c>
-      <c r="H13" s="27">
-        <v>2</v>
-      </c>
-      <c r="I13" s="27">
-        <v>2</v>
-      </c>
-      <c r="J13" s="27">
-        <v>2</v>
-      </c>
-      <c r="K13" s="26">
+      <c r="G13" s="26">
+        <v>2</v>
+      </c>
+      <c r="H13" s="26">
+        <v>2</v>
+      </c>
+      <c r="I13" s="26">
+        <v>2</v>
+      </c>
+      <c r="J13" s="26">
+        <v>2</v>
+      </c>
+      <c r="K13" s="25">
         <v>1</v>
       </c>
-      <c r="L13" s="26">
+      <c r="L13" s="25">
         <v>1</v>
       </c>
-      <c r="M13" s="26">
+      <c r="M13" s="25">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D14" s="31">
+      <c r="D14" s="30">
         <v>5</v>
       </c>
-      <c r="E14" s="30">
+      <c r="E14" s="29">
         <v>4</v>
       </c>
-      <c r="F14" s="30">
+      <c r="F14" s="29">
         <v>4</v>
       </c>
-      <c r="G14" s="29">
+      <c r="G14" s="28">
         <v>6</v>
       </c>
-      <c r="H14" s="28">
+      <c r="H14" s="27">
         <v>3</v>
       </c>
-      <c r="I14" s="26">
+      <c r="I14" s="25">
         <v>1</v>
       </c>
-      <c r="J14" s="25">
+      <c r="J14" s="24">
         <v>0</v>
       </c>
-      <c r="K14" s="25">
+      <c r="K14" s="24">
         <v>0</v>
       </c>
-      <c r="L14" s="27">
-        <v>2</v>
-      </c>
-      <c r="M14" s="27">
+      <c r="L14" s="26">
+        <v>2</v>
+      </c>
+      <c r="M14" s="26">
         <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D15" s="29">
+      <c r="D15" s="28">
         <v>6</v>
       </c>
-      <c r="E15" s="31">
+      <c r="E15" s="30">
         <v>5</v>
       </c>
-      <c r="F15" s="29">
+      <c r="F15" s="28">
         <v>6</v>
       </c>
-      <c r="G15" s="29">
+      <c r="G15" s="28">
         <v>6</v>
       </c>
-      <c r="H15" s="30">
+      <c r="H15" s="29">
         <v>4</v>
       </c>
-      <c r="I15" s="30">
+      <c r="I15" s="29">
         <v>4</v>
       </c>
-      <c r="J15" s="24">
+      <c r="J15" s="23">
         <v>3</v>
       </c>
-      <c r="K15" s="24">
+      <c r="K15" s="23">
         <v>3</v>
       </c>
-      <c r="L15" s="27">
-        <v>2</v>
-      </c>
-      <c r="M15" s="27">
+      <c r="L15" s="26">
+        <v>2</v>
+      </c>
+      <c r="M15" s="26">
         <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="23"/>
-      <c r="K16" s="23"/>
-      <c r="L16" s="23"/>
-      <c r="M16" s="23"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="22"/>
+      <c r="L16" s="22"/>
+      <c r="M16" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1488,13 +1530,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.42578125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1527,18 +1569,18 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" s="1">
         <v>500</v>
       </c>
-      <c r="E4" s="60" t="s">
-        <v>46</v>
-      </c>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="60"/>
+      <c r="E4" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -1547,28 +1589,28 @@
       <c r="B5" s="1">
         <v>0</v>
       </c>
-      <c r="E5" s="55" t="s">
+      <c r="E5" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="52"/>
-      <c r="G5" s="52"/>
-      <c r="H5" s="52"/>
-      <c r="I5" s="53"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="51"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" s="1">
         <v>200</v>
       </c>
-      <c r="E6" s="56" t="s">
+      <c r="E6" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="52"/>
-      <c r="G6" s="52"/>
-      <c r="H6" s="52"/>
-      <c r="I6" s="53"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="50"/>
+      <c r="I6" s="51"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -1577,13 +1619,13 @@
       <c r="B7" s="1">
         <v>100</v>
       </c>
-      <c r="E7" s="56" t="s">
+      <c r="E7" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="49"/>
-      <c r="G7" s="50"/>
-      <c r="H7" s="50"/>
-      <c r="I7" s="51"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="53"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="54"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -1592,132 +1634,132 @@
       <c r="B8" s="1">
         <v>5</v>
       </c>
-      <c r="E8" s="56" t="s">
-        <v>39</v>
-      </c>
-      <c r="F8" s="37"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="39"/>
+      <c r="E8" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="55"/>
+      <c r="G8" s="56"/>
+      <c r="H8" s="56"/>
+      <c r="I8" s="57"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9" s="1">
         <v>6</v>
       </c>
-      <c r="E9" s="56"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="41"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="58"/>
+      <c r="G9" s="59"/>
+      <c r="H9" s="59"/>
+      <c r="I9" s="60"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E10" s="56"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="41"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="58"/>
+      <c r="G10" s="59"/>
+      <c r="H10" s="59"/>
+      <c r="I10" s="60"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E11" s="56"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="36"/>
-      <c r="I11" s="41"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="58"/>
+      <c r="G11" s="59"/>
+      <c r="H11" s="59"/>
+      <c r="I11" s="60"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E12" s="56"/>
-      <c r="F12" s="40"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="41"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="58"/>
+      <c r="G12" s="59"/>
+      <c r="H12" s="59"/>
+      <c r="I12" s="60"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E13" s="56"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="36"/>
-      <c r="H13" s="36"/>
-      <c r="I13" s="41"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="58"/>
+      <c r="G13" s="59"/>
+      <c r="H13" s="59"/>
+      <c r="I13" s="60"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E14" s="56" t="s">
+      <c r="E14" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" s="37"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="39"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E15" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" s="37"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="39"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E16" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="F14" s="46"/>
-      <c r="G14" s="47"/>
-      <c r="H14" s="47"/>
-      <c r="I14" s="48"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E15" s="56" t="s">
+      <c r="F16" s="37"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="39"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E17" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="F15" s="46"/>
-      <c r="G15" s="47"/>
-      <c r="H15" s="47"/>
-      <c r="I15" s="48"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E16" s="56" t="s">
+      <c r="F17" s="37"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="39"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E18" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="F16" s="46"/>
-      <c r="G16" s="47"/>
-      <c r="H16" s="47"/>
-      <c r="I16" s="48"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E17" s="56" t="s">
-        <v>44</v>
-      </c>
-      <c r="F17" s="46"/>
-      <c r="G17" s="47"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="48"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E18" s="57" t="s">
-        <v>45</v>
-      </c>
-      <c r="F18" s="46"/>
-      <c r="G18" s="47"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="48"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="39"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E19" s="56" t="s">
-        <v>40</v>
-      </c>
-      <c r="F19" s="42"/>
-      <c r="G19" s="43"/>
-      <c r="H19" s="43"/>
-      <c r="I19" s="44"/>
+      <c r="E19" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="F19" s="40"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="41"/>
+      <c r="I19" s="42"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E20" s="58"/>
-      <c r="F20" s="45"/>
-      <c r="G20" s="32"/>
-      <c r="H20" s="32"/>
-      <c r="I20" s="33"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="44"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="45"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E21" s="59"/>
-      <c r="F21" s="54"/>
-      <c r="G21" s="34"/>
-      <c r="H21" s="34"/>
-      <c r="I21" s="35"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="47"/>
+      <c r="H21" s="47"/>
+      <c r="I21" s="48"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="C23" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1782,7 +1824,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B29" s="8">
         <v>0.5</v>
@@ -1793,28 +1835,798 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B30" s="13">
+      <c r="B30" s="12">
         <f>SUM(B24:B29)/COUNTA(B24:B29)</f>
         <v>0.58333333333333337</v>
       </c>
-      <c r="C30" s="12">
+      <c r="C30" s="11">
         <f>SUM(C24:C29)</f>
         <v>3633.3333333333335</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="F8:I13"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="F17:I17"/>
     <mergeCell ref="F18:I18"/>
     <mergeCell ref="F19:I21"/>
     <mergeCell ref="E4:I4"/>
     <mergeCell ref="F5:I5"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="F7:I7"/>
+    <mergeCell ref="F8:I13"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="F17:I17"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25:O25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="26" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="1">
+        <v>500</v>
+      </c>
+      <c r="E4" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="K4" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="L4" s="49"/>
+      <c r="M4" s="49"/>
+      <c r="N4" s="49"/>
+      <c r="O4" s="49"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="50" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5" s="50"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="51"/>
+      <c r="K5" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="L5" s="50" t="s">
+        <v>46</v>
+      </c>
+      <c r="M5" s="50"/>
+      <c r="N5" s="50"/>
+      <c r="O5" s="51"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="1">
+        <v>200</v>
+      </c>
+      <c r="E6" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="50">
+        <v>125</v>
+      </c>
+      <c r="G6" s="50"/>
+      <c r="H6" s="50"/>
+      <c r="I6" s="51"/>
+      <c r="K6" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="L6" s="50" t="s">
+        <v>49</v>
+      </c>
+      <c r="M6" s="50"/>
+      <c r="N6" s="50"/>
+      <c r="O6" s="51"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1">
+        <v>100</v>
+      </c>
+      <c r="E7" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="52">
+        <v>3</v>
+      </c>
+      <c r="G7" s="53"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="54"/>
+      <c r="K7" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="L7" s="52">
+        <v>0</v>
+      </c>
+      <c r="M7" s="53"/>
+      <c r="N7" s="53"/>
+      <c r="O7" s="54"/>
+    </row>
+    <row r="8" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1">
+        <v>5</v>
+      </c>
+      <c r="E8" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="55" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" s="56"/>
+      <c r="H8" s="56"/>
+      <c r="I8" s="57"/>
+      <c r="K8" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="L8" s="55" t="s">
+        <v>48</v>
+      </c>
+      <c r="M8" s="56"/>
+      <c r="N8" s="56"/>
+      <c r="O8" s="57"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="1">
+        <v>6</v>
+      </c>
+      <c r="E9" s="32"/>
+      <c r="F9" s="58"/>
+      <c r="G9" s="59"/>
+      <c r="H9" s="59"/>
+      <c r="I9" s="60"/>
+      <c r="K9" s="32"/>
+      <c r="L9" s="58"/>
+      <c r="M9" s="59"/>
+      <c r="N9" s="59"/>
+      <c r="O9" s="60"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E10" s="32"/>
+      <c r="F10" s="58"/>
+      <c r="G10" s="59"/>
+      <c r="H10" s="59"/>
+      <c r="I10" s="60"/>
+      <c r="K10" s="32"/>
+      <c r="L10" s="58"/>
+      <c r="M10" s="59"/>
+      <c r="N10" s="59"/>
+      <c r="O10" s="60"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E11" s="32"/>
+      <c r="F11" s="58"/>
+      <c r="G11" s="59"/>
+      <c r="H11" s="59"/>
+      <c r="I11" s="60"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="58"/>
+      <c r="M11" s="59"/>
+      <c r="N11" s="59"/>
+      <c r="O11" s="60"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E12" s="32"/>
+      <c r="F12" s="58"/>
+      <c r="G12" s="59"/>
+      <c r="H12" s="59"/>
+      <c r="I12" s="60"/>
+      <c r="K12" s="32"/>
+      <c r="L12" s="58"/>
+      <c r="M12" s="59"/>
+      <c r="N12" s="59"/>
+      <c r="O12" s="60"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E13" s="32"/>
+      <c r="F13" s="58"/>
+      <c r="G13" s="59"/>
+      <c r="H13" s="59"/>
+      <c r="I13" s="60"/>
+      <c r="K13" s="32"/>
+      <c r="L13" s="58"/>
+      <c r="M13" s="59"/>
+      <c r="N13" s="59"/>
+      <c r="O13" s="60"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E14" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" s="37">
+        <v>4</v>
+      </c>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="39"/>
+      <c r="K14" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="L14" s="37">
+        <v>6</v>
+      </c>
+      <c r="M14" s="38"/>
+      <c r="N14" s="38"/>
+      <c r="O14" s="39"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E15" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" s="37"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="39"/>
+      <c r="K15" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="L15" s="37"/>
+      <c r="M15" s="38"/>
+      <c r="N15" s="38"/>
+      <c r="O15" s="39"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E16" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="37"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="39"/>
+      <c r="K16" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="L16" s="37"/>
+      <c r="M16" s="38"/>
+      <c r="N16" s="38"/>
+      <c r="O16" s="39"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E17" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="F17" s="37"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="39"/>
+      <c r="K17" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="L17" s="37"/>
+      <c r="M17" s="38"/>
+      <c r="N17" s="38"/>
+      <c r="O17" s="39"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E18" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="F18" s="37"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="39"/>
+      <c r="K18" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="L18" s="37"/>
+      <c r="M18" s="38"/>
+      <c r="N18" s="38"/>
+      <c r="O18" s="39"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E19" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="F19" s="40"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="41"/>
+      <c r="I19" s="42"/>
+      <c r="K19" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="L19" s="40"/>
+      <c r="M19" s="41"/>
+      <c r="N19" s="41"/>
+      <c r="O19" s="42"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E20" s="34"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="44"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="45"/>
+      <c r="K20" s="34"/>
+      <c r="L20" s="43"/>
+      <c r="M20" s="44"/>
+      <c r="N20" s="44"/>
+      <c r="O20" s="45"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E21" s="35"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="47"/>
+      <c r="H21" s="47"/>
+      <c r="I21" s="48"/>
+      <c r="K21" s="35"/>
+      <c r="L21" s="46"/>
+      <c r="M21" s="47"/>
+      <c r="N21" s="47"/>
+      <c r="O21" s="48"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E23" s="49" t="s">
+        <v>52</v>
+      </c>
+      <c r="F23" s="49"/>
+      <c r="G23" s="49"/>
+      <c r="H23" s="49"/>
+      <c r="I23" s="49"/>
+      <c r="K23" s="49" t="s">
+        <v>54</v>
+      </c>
+      <c r="L23" s="49"/>
+      <c r="M23" s="49"/>
+      <c r="N23" s="49"/>
+      <c r="O23" s="49"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="8">
+        <v>0.75</v>
+      </c>
+      <c r="C24" s="3">
+        <f>Constants!B2*Constants!F2*B8*Tactician!B24</f>
+        <v>375</v>
+      </c>
+      <c r="E24" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="G24" s="50"/>
+      <c r="H24" s="50"/>
+      <c r="I24" s="51"/>
+      <c r="K24" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="L24" s="50" t="s">
+        <v>55</v>
+      </c>
+      <c r="M24" s="50"/>
+      <c r="N24" s="50"/>
+      <c r="O24" s="51"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" s="8">
+        <v>0.75</v>
+      </c>
+      <c r="C25" s="3">
+        <f>B6+B7*Constants!B2*Constants!F3*B25</f>
+        <v>950</v>
+      </c>
+      <c r="E25" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="50">
+        <v>50</v>
+      </c>
+      <c r="G25" s="50"/>
+      <c r="H25" s="50"/>
+      <c r="I25" s="51"/>
+      <c r="K25" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="L25" s="50">
+        <v>75</v>
+      </c>
+      <c r="M25" s="50"/>
+      <c r="N25" s="50"/>
+      <c r="O25" s="51"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" s="8">
+        <v>0.75</v>
+      </c>
+      <c r="C26" s="3">
+        <f>Constants!F4*B4*B26</f>
+        <v>1125</v>
+      </c>
+      <c r="E26" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="52">
+        <v>1</v>
+      </c>
+      <c r="G26" s="53"/>
+      <c r="H26" s="53"/>
+      <c r="I26" s="54"/>
+      <c r="K26" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="L26" s="52">
+        <v>2</v>
+      </c>
+      <c r="M26" s="53"/>
+      <c r="N26" s="53"/>
+      <c r="O26" s="54"/>
+    </row>
+    <row r="27" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="C27" s="3">
+        <f>Constants!F5*B4*B27</f>
+        <v>250</v>
+      </c>
+      <c r="E27" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="F27" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="G27" s="56"/>
+      <c r="H27" s="56"/>
+      <c r="I27" s="57"/>
+      <c r="K27" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="L27" s="55" t="s">
+        <v>56</v>
+      </c>
+      <c r="M27" s="56"/>
+      <c r="N27" s="56"/>
+      <c r="O27" s="57"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="C28" s="3">
+        <f>Constants!F6*Constants!B2*B28</f>
+        <v>500</v>
+      </c>
+      <c r="E28" s="32"/>
+      <c r="F28" s="58"/>
+      <c r="G28" s="59"/>
+      <c r="H28" s="59"/>
+      <c r="I28" s="60"/>
+      <c r="K28" s="32"/>
+      <c r="L28" s="58"/>
+      <c r="M28" s="59"/>
+      <c r="N28" s="59"/>
+      <c r="O28" s="60"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="C29" s="9">
+        <f>B29*(Constants!F7*(1+Constants!B2/Constants!B3))</f>
+        <v>433.33333333333337</v>
+      </c>
+      <c r="E29" s="32"/>
+      <c r="F29" s="58"/>
+      <c r="G29" s="59"/>
+      <c r="H29" s="59"/>
+      <c r="I29" s="60"/>
+      <c r="K29" s="32"/>
+      <c r="L29" s="58"/>
+      <c r="M29" s="59"/>
+      <c r="N29" s="59"/>
+      <c r="O29" s="60"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B30" s="12">
+        <f>SUM(B24:B29)/COUNTA(B24:B29)</f>
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C30" s="11">
+        <f>SUM(C24:C29)</f>
+        <v>3633.3333333333335</v>
+      </c>
+      <c r="E30" s="32"/>
+      <c r="F30" s="58"/>
+      <c r="G30" s="59"/>
+      <c r="H30" s="59"/>
+      <c r="I30" s="60"/>
+      <c r="K30" s="32"/>
+      <c r="L30" s="58"/>
+      <c r="M30" s="59"/>
+      <c r="N30" s="59"/>
+      <c r="O30" s="60"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E31" s="32"/>
+      <c r="F31" s="58"/>
+      <c r="G31" s="59"/>
+      <c r="H31" s="59"/>
+      <c r="I31" s="60"/>
+      <c r="K31" s="32"/>
+      <c r="L31" s="58"/>
+      <c r="M31" s="59"/>
+      <c r="N31" s="59"/>
+      <c r="O31" s="60"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E32" s="32"/>
+      <c r="F32" s="58"/>
+      <c r="G32" s="59"/>
+      <c r="H32" s="59"/>
+      <c r="I32" s="60"/>
+      <c r="K32" s="32"/>
+      <c r="L32" s="58"/>
+      <c r="M32" s="59"/>
+      <c r="N32" s="59"/>
+      <c r="O32" s="60"/>
+    </row>
+    <row r="33" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E33" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="F33" s="37">
+        <v>5</v>
+      </c>
+      <c r="G33" s="38"/>
+      <c r="H33" s="38"/>
+      <c r="I33" s="39"/>
+      <c r="K33" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="L33" s="37">
+        <v>5</v>
+      </c>
+      <c r="M33" s="38"/>
+      <c r="N33" s="38"/>
+      <c r="O33" s="39"/>
+    </row>
+    <row r="34" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E34" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="F34" s="37">
+        <v>80</v>
+      </c>
+      <c r="G34" s="38"/>
+      <c r="H34" s="38"/>
+      <c r="I34" s="39"/>
+      <c r="K34" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="L34" s="37">
+        <v>80</v>
+      </c>
+      <c r="M34" s="38"/>
+      <c r="N34" s="38"/>
+      <c r="O34" s="39"/>
+    </row>
+    <row r="35" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E35" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="F35" s="37"/>
+      <c r="G35" s="38"/>
+      <c r="H35" s="38"/>
+      <c r="I35" s="39"/>
+      <c r="K35" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="L35" s="37"/>
+      <c r="M35" s="38"/>
+      <c r="N35" s="38"/>
+      <c r="O35" s="39"/>
+    </row>
+    <row r="36" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E36" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="F36" s="37"/>
+      <c r="G36" s="38"/>
+      <c r="H36" s="38"/>
+      <c r="I36" s="39"/>
+      <c r="K36" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="L36" s="37"/>
+      <c r="M36" s="38"/>
+      <c r="N36" s="38"/>
+      <c r="O36" s="39"/>
+    </row>
+    <row r="37" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E37" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="F37" s="37"/>
+      <c r="G37" s="38"/>
+      <c r="H37" s="38"/>
+      <c r="I37" s="39"/>
+      <c r="K37" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="L37" s="37"/>
+      <c r="M37" s="38"/>
+      <c r="N37" s="38"/>
+      <c r="O37" s="39"/>
+    </row>
+    <row r="38" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E38" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="F38" s="40"/>
+      <c r="G38" s="41"/>
+      <c r="H38" s="41"/>
+      <c r="I38" s="42"/>
+      <c r="K38" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="L38" s="40"/>
+      <c r="M38" s="41"/>
+      <c r="N38" s="41"/>
+      <c r="O38" s="42"/>
+    </row>
+    <row r="39" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E39" s="34"/>
+      <c r="F39" s="43"/>
+      <c r="G39" s="44"/>
+      <c r="H39" s="44"/>
+      <c r="I39" s="45"/>
+      <c r="K39" s="34"/>
+      <c r="L39" s="43"/>
+      <c r="M39" s="44"/>
+      <c r="N39" s="44"/>
+      <c r="O39" s="45"/>
+    </row>
+    <row r="40" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E40" s="35"/>
+      <c r="F40" s="46"/>
+      <c r="G40" s="47"/>
+      <c r="H40" s="47"/>
+      <c r="I40" s="48"/>
+      <c r="K40" s="35"/>
+      <c r="L40" s="46"/>
+      <c r="M40" s="47"/>
+      <c r="N40" s="47"/>
+      <c r="O40" s="48"/>
+    </row>
+  </sheetData>
+  <mergeCells count="44">
+    <mergeCell ref="L36:O36"/>
+    <mergeCell ref="L37:O37"/>
+    <mergeCell ref="L38:O40"/>
+    <mergeCell ref="L26:O26"/>
+    <mergeCell ref="L27:O32"/>
+    <mergeCell ref="L33:O33"/>
+    <mergeCell ref="L34:O34"/>
+    <mergeCell ref="L35:O35"/>
+    <mergeCell ref="E4:I4"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="F7:I7"/>
+    <mergeCell ref="F8:I13"/>
+    <mergeCell ref="K4:O4"/>
+    <mergeCell ref="L5:O5"/>
+    <mergeCell ref="L6:O6"/>
+    <mergeCell ref="L7:O7"/>
+    <mergeCell ref="L8:O13"/>
+    <mergeCell ref="F33:I33"/>
+    <mergeCell ref="L14:O14"/>
+    <mergeCell ref="L15:O15"/>
+    <mergeCell ref="L16:O16"/>
+    <mergeCell ref="L17:O17"/>
+    <mergeCell ref="L18:O18"/>
+    <mergeCell ref="L19:O21"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="F19:I21"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="K23:O23"/>
+    <mergeCell ref="L24:O24"/>
+    <mergeCell ref="L25:O25"/>
+    <mergeCell ref="E23:I23"/>
+    <mergeCell ref="F24:I24"/>
+    <mergeCell ref="F25:I25"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="F27:I32"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="F36:I36"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="F38:I40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Initial brief of second character
</commit_message>
<xml_diff>
--- a/Documents/Balance.xlsx
+++ b/Documents/Balance.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13275" tabRatio="462" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13275" tabRatio="462" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Analysis" sheetId="3" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="Example_Map" sheetId="2" r:id="rId3"/>
     <sheet name="Average_Character_Template" sheetId="1" r:id="rId4"/>
     <sheet name="Tactician" sheetId="5" r:id="rId5"/>
+    <sheet name="Electrifier" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="67">
   <si>
     <t>Width:</t>
   </si>
@@ -205,6 +206,30 @@
   </si>
   <si>
     <t>Onclass Utility</t>
+  </si>
+  <si>
+    <t>All energy</t>
+  </si>
+  <si>
+    <t>0.5</t>
+  </si>
+  <si>
+    <t>Consumes all energy to deal {P1} damage for each energy point spent in a {P2} radius around the character. If 100 or more energy is spent, the movement speed energy cost of all opponents affected is increased by {P3} during their next round. If 200 or more energy is spent, the character gains a shield with {P4} health for each energy spent which lasts {P5} turns or until destroyed.</t>
+  </si>
+  <si>
+    <t>0.1</t>
+  </si>
+  <si>
+    <t>Restoring Stasis</t>
+  </si>
+  <si>
+    <t>Orbital Shifter</t>
+  </si>
+  <si>
+    <t>Target two tiles in {P1} radius. Swap the height of both tiles. If there is a character on the first tile, teleport it to the other tile. If a character has been moved, ? takes {P2} damage for each tile moved.</t>
+  </si>
+  <si>
+    <t>Restores {P1} energy, but disables the 'Movement' ability during your next turn.</t>
   </si>
 </sst>
 </file>
@@ -459,7 +484,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -613,6 +638,15 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1870,8 +1904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2253,11 +2287,11 @@
         <v>21</v>
       </c>
       <c r="B24" s="8">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="C24" s="3">
         <f>Constants!B2*Constants!F2*B8*Tactician!B24</f>
-        <v>375</v>
+        <v>250</v>
       </c>
       <c r="E24" s="31" t="s">
         <v>9</v>
@@ -2283,11 +2317,11 @@
         <v>16</v>
       </c>
       <c r="B25" s="8">
-        <v>0.75</v>
+        <v>0.9</v>
       </c>
       <c r="C25" s="3">
         <f>B6+B7*Constants!B2*Constants!F3*B25</f>
-        <v>950</v>
+        <v>1100</v>
       </c>
       <c r="E25" s="32" t="s">
         <v>10</v>
@@ -2313,11 +2347,11 @@
         <v>17</v>
       </c>
       <c r="B26" s="8">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="C26" s="3">
         <f>Constants!F4*B4*B26</f>
-        <v>1125</v>
+        <v>1200</v>
       </c>
       <c r="E26" s="32" t="s">
         <v>11</v>
@@ -2343,11 +2377,11 @@
         <v>20</v>
       </c>
       <c r="B27" s="8">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="C27" s="3">
         <f>Constants!F5*B4*B27</f>
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="E27" s="32" t="s">
         <v>45</v>
@@ -2373,11 +2407,11 @@
         <v>22</v>
       </c>
       <c r="B28" s="8">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="C28" s="3">
         <f>Constants!F6*Constants!B2*B28</f>
-        <v>500</v>
+        <v>750</v>
       </c>
       <c r="E28" s="32"/>
       <c r="F28" s="58"/>
@@ -2395,11 +2429,11 @@
         <v>25</v>
       </c>
       <c r="B29" s="8">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="C29" s="9">
         <f>B29*(Constants!F7*(1+Constants!B2/Constants!B3))</f>
-        <v>433.33333333333337</v>
+        <v>173.33333333333337</v>
       </c>
       <c r="E29" s="32"/>
       <c r="F29" s="58"/>
@@ -2415,11 +2449,11 @@
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B30" s="12">
         <f>SUM(B24:B29)/COUNTA(B24:B29)</f>
-        <v>0.58333333333333337</v>
+        <v>0.52500000000000002</v>
       </c>
       <c r="C30" s="11">
         <f>SUM(C24:C29)</f>
-        <v>3633.3333333333335</v>
+        <v>3473.3333333333335</v>
       </c>
       <c r="E30" s="32"/>
       <c r="F30" s="58"/>
@@ -2586,16 +2620,24 @@
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="F34:I34"/>
-    <mergeCell ref="F35:I35"/>
-    <mergeCell ref="F36:I36"/>
-    <mergeCell ref="F37:I37"/>
-    <mergeCell ref="F38:I40"/>
-    <mergeCell ref="E23:I23"/>
-    <mergeCell ref="F24:I24"/>
-    <mergeCell ref="F25:I25"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="F27:I32"/>
+    <mergeCell ref="L36:O36"/>
+    <mergeCell ref="L37:O37"/>
+    <mergeCell ref="L38:O40"/>
+    <mergeCell ref="L26:O26"/>
+    <mergeCell ref="L27:O32"/>
+    <mergeCell ref="L33:O33"/>
+    <mergeCell ref="L34:O34"/>
+    <mergeCell ref="L35:O35"/>
+    <mergeCell ref="E4:I4"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="F7:I7"/>
+    <mergeCell ref="F8:I13"/>
+    <mergeCell ref="K4:O4"/>
+    <mergeCell ref="L5:O5"/>
+    <mergeCell ref="L6:O6"/>
+    <mergeCell ref="L7:O7"/>
+    <mergeCell ref="L8:O13"/>
     <mergeCell ref="F33:I33"/>
     <mergeCell ref="L14:O14"/>
     <mergeCell ref="L15:O15"/>
@@ -2612,6 +2654,648 @@
     <mergeCell ref="K23:O23"/>
     <mergeCell ref="L24:O24"/>
     <mergeCell ref="L25:O25"/>
+    <mergeCell ref="E23:I23"/>
+    <mergeCell ref="F24:I24"/>
+    <mergeCell ref="F25:I25"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="F27:I32"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="F36:I36"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="F38:I40"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="26" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="1">
+        <v>425</v>
+      </c>
+      <c r="E4" s="49" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="K4" s="49" t="s">
+        <v>52</v>
+      </c>
+      <c r="L4" s="49"/>
+      <c r="M4" s="49"/>
+      <c r="N4" s="49"/>
+      <c r="O4" s="49"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="50" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5" s="50"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="51"/>
+      <c r="K5" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="L5" s="50" t="s">
+        <v>55</v>
+      </c>
+      <c r="M5" s="50"/>
+      <c r="N5" s="50"/>
+      <c r="O5" s="51"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="1">
+        <v>250</v>
+      </c>
+      <c r="E6" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="50">
+        <v>50</v>
+      </c>
+      <c r="G6" s="50"/>
+      <c r="H6" s="50"/>
+      <c r="I6" s="51"/>
+      <c r="K6" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="L6" s="50" t="s">
+        <v>59</v>
+      </c>
+      <c r="M6" s="50"/>
+      <c r="N6" s="50"/>
+      <c r="O6" s="51"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1">
+        <v>100</v>
+      </c>
+      <c r="E7" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="52">
+        <v>2</v>
+      </c>
+      <c r="G7" s="53"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="54"/>
+      <c r="K7" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="L7" s="52">
+        <v>1</v>
+      </c>
+      <c r="M7" s="53"/>
+      <c r="N7" s="53"/>
+      <c r="O7" s="54"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1">
+        <v>5</v>
+      </c>
+      <c r="E8" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="55" t="s">
+        <v>65</v>
+      </c>
+      <c r="G8" s="56"/>
+      <c r="H8" s="56"/>
+      <c r="I8" s="57"/>
+      <c r="K8" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="L8" s="55" t="s">
+        <v>61</v>
+      </c>
+      <c r="M8" s="56"/>
+      <c r="N8" s="56"/>
+      <c r="O8" s="57"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="1">
+        <v>6</v>
+      </c>
+      <c r="E9" s="32"/>
+      <c r="F9" s="58"/>
+      <c r="G9" s="59"/>
+      <c r="H9" s="59"/>
+      <c r="I9" s="60"/>
+      <c r="K9" s="32"/>
+      <c r="L9" s="58"/>
+      <c r="M9" s="59"/>
+      <c r="N9" s="59"/>
+      <c r="O9" s="60"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E10" s="32"/>
+      <c r="F10" s="58"/>
+      <c r="G10" s="59"/>
+      <c r="H10" s="59"/>
+      <c r="I10" s="60"/>
+      <c r="K10" s="32"/>
+      <c r="L10" s="58"/>
+      <c r="M10" s="59"/>
+      <c r="N10" s="59"/>
+      <c r="O10" s="60"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E11" s="32"/>
+      <c r="F11" s="58"/>
+      <c r="G11" s="59"/>
+      <c r="H11" s="59"/>
+      <c r="I11" s="60"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="58"/>
+      <c r="M11" s="59"/>
+      <c r="N11" s="59"/>
+      <c r="O11" s="60"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E12" s="32"/>
+      <c r="F12" s="58"/>
+      <c r="G12" s="59"/>
+      <c r="H12" s="59"/>
+      <c r="I12" s="60"/>
+      <c r="K12" s="32"/>
+      <c r="L12" s="58"/>
+      <c r="M12" s="59"/>
+      <c r="N12" s="59"/>
+      <c r="O12" s="60"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E13" s="32"/>
+      <c r="F13" s="61"/>
+      <c r="G13" s="62"/>
+      <c r="H13" s="62"/>
+      <c r="I13" s="63"/>
+      <c r="K13" s="32"/>
+      <c r="L13" s="58"/>
+      <c r="M13" s="59"/>
+      <c r="N13" s="59"/>
+      <c r="O13" s="60"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E14" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" s="52">
+        <v>4</v>
+      </c>
+      <c r="G14" s="53"/>
+      <c r="H14" s="53"/>
+      <c r="I14" s="54"/>
+      <c r="K14" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="L14" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="M14" s="38"/>
+      <c r="N14" s="38"/>
+      <c r="O14" s="39"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E15" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" s="52">
+        <v>5</v>
+      </c>
+      <c r="G15" s="53"/>
+      <c r="H15" s="53"/>
+      <c r="I15" s="54"/>
+      <c r="K15" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="L15" s="37">
+        <v>3</v>
+      </c>
+      <c r="M15" s="38"/>
+      <c r="N15" s="38"/>
+      <c r="O15" s="39"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E16" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="52"/>
+      <c r="G16" s="53"/>
+      <c r="H16" s="53"/>
+      <c r="I16" s="54"/>
+      <c r="K16" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="L16" s="37">
+        <v>1</v>
+      </c>
+      <c r="M16" s="38"/>
+      <c r="N16" s="38"/>
+      <c r="O16" s="39"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E17" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="F17" s="52"/>
+      <c r="G17" s="53"/>
+      <c r="H17" s="53"/>
+      <c r="I17" s="54"/>
+      <c r="K17" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="L17" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="M17" s="38"/>
+      <c r="N17" s="38"/>
+      <c r="O17" s="39"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E18" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="F18" s="52"/>
+      <c r="G18" s="53"/>
+      <c r="H18" s="53"/>
+      <c r="I18" s="54"/>
+      <c r="K18" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="L18" s="37">
+        <v>2</v>
+      </c>
+      <c r="M18" s="38"/>
+      <c r="N18" s="38"/>
+      <c r="O18" s="39"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E19" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="F19" s="40"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="41"/>
+      <c r="I19" s="42"/>
+      <c r="K19" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="L19" s="40"/>
+      <c r="M19" s="41"/>
+      <c r="N19" s="41"/>
+      <c r="O19" s="42"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E20" s="34"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="44"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="45"/>
+      <c r="K20" s="34"/>
+      <c r="L20" s="43"/>
+      <c r="M20" s="44"/>
+      <c r="N20" s="44"/>
+      <c r="O20" s="45"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E21" s="35"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="47"/>
+      <c r="H21" s="47"/>
+      <c r="I21" s="48"/>
+      <c r="K21" s="35"/>
+      <c r="L21" s="46"/>
+      <c r="M21" s="47"/>
+      <c r="N21" s="47"/>
+      <c r="O21" s="48"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E23" s="49" t="s">
+        <v>54</v>
+      </c>
+      <c r="F23" s="49"/>
+      <c r="G23" s="49"/>
+      <c r="H23" s="49"/>
+      <c r="I23" s="49"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="C24" s="3">
+        <f>Constants!B2*Constants!F2*B8*Electrifier!B24</f>
+        <v>250</v>
+      </c>
+      <c r="E24" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="50" t="s">
+        <v>63</v>
+      </c>
+      <c r="G24" s="50"/>
+      <c r="H24" s="50"/>
+      <c r="I24" s="51"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" s="8">
+        <v>0.9</v>
+      </c>
+      <c r="C25" s="3">
+        <f>B6+B7*Constants!B2*Constants!F3*B25</f>
+        <v>1150</v>
+      </c>
+      <c r="E25" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="50">
+        <v>0</v>
+      </c>
+      <c r="G25" s="50"/>
+      <c r="H25" s="50"/>
+      <c r="I25" s="51"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="C26" s="3">
+        <f>Constants!F4*B4*B26</f>
+        <v>637.5</v>
+      </c>
+      <c r="E26" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="52">
+        <v>2</v>
+      </c>
+      <c r="G26" s="53"/>
+      <c r="H26" s="53"/>
+      <c r="I26" s="54"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="C27" s="3">
+        <f>Constants!F5*B4*B27</f>
+        <v>340</v>
+      </c>
+      <c r="E27" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="F27" s="55" t="s">
+        <v>66</v>
+      </c>
+      <c r="G27" s="56"/>
+      <c r="H27" s="56"/>
+      <c r="I27" s="57"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" s="8">
+        <v>0.9</v>
+      </c>
+      <c r="C28" s="3">
+        <f>Constants!F6*Constants!B2*B28</f>
+        <v>900</v>
+      </c>
+      <c r="E28" s="32"/>
+      <c r="F28" s="58"/>
+      <c r="G28" s="59"/>
+      <c r="H28" s="59"/>
+      <c r="I28" s="60"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="C29" s="9">
+        <f>B29*(Constants!F7*(1+Constants!B2/Constants!B3))</f>
+        <v>173.33333333333337</v>
+      </c>
+      <c r="E29" s="32"/>
+      <c r="F29" s="58"/>
+      <c r="G29" s="59"/>
+      <c r="H29" s="59"/>
+      <c r="I29" s="60"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B30" s="12">
+        <f>SUM(B24:B29)/COUNTA(B24:B29)</f>
+        <v>0.56666666666666665</v>
+      </c>
+      <c r="C30" s="11">
+        <f>SUM(C24:C29)</f>
+        <v>3450.8333333333335</v>
+      </c>
+      <c r="E30" s="32"/>
+      <c r="F30" s="58"/>
+      <c r="G30" s="59"/>
+      <c r="H30" s="59"/>
+      <c r="I30" s="60"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E31" s="32"/>
+      <c r="F31" s="58"/>
+      <c r="G31" s="59"/>
+      <c r="H31" s="59"/>
+      <c r="I31" s="60"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E32" s="32"/>
+      <c r="F32" s="58"/>
+      <c r="G32" s="59"/>
+      <c r="H32" s="59"/>
+      <c r="I32" s="60"/>
+    </row>
+    <row r="33" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E33" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="F33" s="37">
+        <v>50</v>
+      </c>
+      <c r="G33" s="38"/>
+      <c r="H33" s="38"/>
+      <c r="I33" s="39"/>
+    </row>
+    <row r="34" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E34" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="F34" s="37"/>
+      <c r="G34" s="38"/>
+      <c r="H34" s="38"/>
+      <c r="I34" s="39"/>
+    </row>
+    <row r="35" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E35" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="F35" s="37"/>
+      <c r="G35" s="38"/>
+      <c r="H35" s="38"/>
+      <c r="I35" s="39"/>
+    </row>
+    <row r="36" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E36" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="F36" s="37"/>
+      <c r="G36" s="38"/>
+      <c r="H36" s="38"/>
+      <c r="I36" s="39"/>
+    </row>
+    <row r="37" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E37" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="F37" s="37"/>
+      <c r="G37" s="38"/>
+      <c r="H37" s="38"/>
+      <c r="I37" s="39"/>
+    </row>
+    <row r="38" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E38" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="F38" s="40"/>
+      <c r="G38" s="41"/>
+      <c r="H38" s="41"/>
+      <c r="I38" s="42"/>
+    </row>
+    <row r="39" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E39" s="34"/>
+      <c r="F39" s="43"/>
+      <c r="G39" s="44"/>
+      <c r="H39" s="44"/>
+      <c r="I39" s="45"/>
+    </row>
+    <row r="40" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E40" s="35"/>
+      <c r="F40" s="46"/>
+      <c r="G40" s="47"/>
+      <c r="H40" s="47"/>
+      <c r="I40" s="48"/>
+    </row>
+  </sheetData>
+  <mergeCells count="33">
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="F36:I36"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="F38:I40"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="E23:I23"/>
+    <mergeCell ref="F24:I24"/>
+    <mergeCell ref="F25:I25"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="F27:I32"/>
+    <mergeCell ref="F33:I33"/>
+    <mergeCell ref="L15:O15"/>
+    <mergeCell ref="L16:O16"/>
+    <mergeCell ref="L17:O17"/>
+    <mergeCell ref="L18:O18"/>
+    <mergeCell ref="L19:O21"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="F19:I21"/>
     <mergeCell ref="K4:O4"/>
     <mergeCell ref="L5:O5"/>
     <mergeCell ref="L6:O6"/>
@@ -2622,14 +3306,7 @@
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="F7:I7"/>
     <mergeCell ref="F8:I13"/>
-    <mergeCell ref="L36:O36"/>
-    <mergeCell ref="L37:O37"/>
-    <mergeCell ref="L38:O40"/>
-    <mergeCell ref="L26:O26"/>
-    <mergeCell ref="L27:O32"/>
-    <mergeCell ref="L33:O33"/>
-    <mergeCell ref="L34:O34"/>
-    <mergeCell ref="L35:O35"/>
+    <mergeCell ref="L14:O14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>